<commit_message>
Updated the Effort Estimation sheet
</commit_message>
<xml_diff>
--- a/EffortEstimation/EffortEstimationFile.xlsx
+++ b/EffortEstimation/EffortEstimationFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SypIonciProject\master\project-proposal-allround-manager-prototype-name\EffortEstimation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\SYP\Allround Manager\project-proposal-allround-manager-prototype-name\EffortEstimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989648EA-E0B6-43A2-BC29-80EFE9ED82FE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BA52CD-899E-46EE-A51A-6F4474B4EF84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{A86B2A40-5864-4E44-B1D9-9A99AF58399A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="12060" xr2:uid="{A86B2A40-5864-4E44-B1D9-9A99AF58399A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>2.5h</t>
+  </si>
+  <si>
+    <t>Make a simple Adobe Xd design</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,14 +631,18 @@
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5">
+        <v>13</v>
+      </c>
       <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -797,12 +804,24 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>

</xml_diff>